<commit_message>
Adição das dependências lógicas
</commit_message>
<xml_diff>
--- a/Dependências/action-center-platform/formalized_tasks_action-center-platform.git.xlsx
+++ b/Dependências/action-center-platform/formalized_tasks_action-center-platform.git.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Pesquisa TAITI\Dependências\action-center-platform\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -238,8 +243,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,18 +315,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -359,9 +372,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,9 +406,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,9 +441,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -602,14 +617,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +668,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -688,7 +709,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -729,7 +750,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -770,7 +791,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -811,7 +832,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -852,7 +873,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -893,7 +914,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -934,7 +955,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -975,7 +996,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1016,7 +1037,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1057,7 +1078,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1098,7 +1119,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1139,7 +1160,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1180,7 +1201,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1221,7 +1242,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1262,7 +1283,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1303,7 +1324,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>

</xml_diff>